<commit_message>
updated the dpi of the graphs and tables
</commit_message>
<xml_diff>
--- a/assets/SIT_User_Study.xlsx
+++ b/assets/SIT_User_Study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\krispy_noodles\SIT_Chatbot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6EC452-F0E8-4524-8503-C39C9849D070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B737DD35-FA7A-49C4-BFD8-C6B173E24916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-4190" windowWidth="25820" windowHeight="15500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Question 1" sheetId="1" r:id="rId1"/>
@@ -205,9 +205,6 @@
     <t>Faster and I dont have to look through so much bullshit and I can just type key words easy</t>
   </si>
   <si>
-    <t>It is so much more convienent, you just need to type in key words and you dont have to squnich your eyes to look for everything on the website</t>
-  </si>
-  <si>
     <t>It just goes direct to the point, you dont need to go through pages where you think that the information is there but it is not</t>
   </si>
   <si>
@@ -238,9 +235,6 @@
     <t>SIT Students?</t>
   </si>
   <si>
-    <t>The wbesite is very confusing in general and the way that is it categorise can be quite confusing for example when looking for an email about admission, why isit not under the admission tab but rather in the contact us page</t>
-  </si>
-  <si>
     <t>I really prefer the chatbot as it I get my question answered alot faster than the website</t>
   </si>
   <si>
@@ -293,6 +287,12 @@
   </si>
   <si>
     <t>Depth of Information</t>
+  </si>
+  <si>
+    <t>It is so much more convenient, you just need to type in key words and you dont have to squnich your eyes to look for everything on the website</t>
+  </si>
+  <si>
+    <t>The wbesite is very confusing in general and the way that is it categorized can be quite confusing for example when looking for an email about admission, why isit not under the admission tab but rather in the contact us page</t>
   </si>
 </sst>
 </file>
@@ -667,10 +667,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1311,10 +1311,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1955,10 +1955,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2597,10 +2597,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -3239,10 +3239,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -3853,9 +3853,9 @@
   </sheetPr>
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3864,13 +3864,13 @@
     <col min="3" max="3" width="27.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
     <col min="5" max="5" width="22.140625" customWidth="1"/>
-    <col min="6" max="6" width="80.7109375" customWidth="1"/>
+    <col min="6" max="6" width="102.140625" customWidth="1"/>
     <col min="7" max="7" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>36</v>
@@ -3885,7 +3885,7 @@
         <v>39</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3905,10 +3905,10 @@
         <v>41</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3928,10 +3928,10 @@
         <v>41</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3951,10 +3951,10 @@
         <v>41</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3977,7 +3977,7 @@
         <v>43</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4000,7 +4000,7 @@
         <v>44</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -4023,7 +4023,7 @@
         <v>45</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4046,7 +4046,7 @@
         <v>46</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -4069,7 +4069,7 @@
         <v>47</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4092,7 +4092,7 @@
         <v>49</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -4115,10 +4115,10 @@
         <v>50</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -4138,10 +4138,10 @@
         <v>51</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -4161,7 +4161,7 @@
         <v>52</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4184,10 +4184,10 @@
         <v>53</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -4204,10 +4204,10 @@
         <v>41</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4230,7 +4230,7 @@
         <v>54</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -4250,10 +4250,10 @@
         <v>41</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -4273,10 +4273,10 @@
         <v>41</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4296,10 +4296,10 @@
         <v>48</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4319,10 +4319,10 @@
         <v>41</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4342,10 +4342,10 @@
         <v>48</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -4365,10 +4365,10 @@
         <v>41</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4388,10 +4388,10 @@
         <v>48</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -4411,45 +4411,45 @@
         <v>41</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>